<commit_message>
Initial commit: Capstone logistics management system
</commit_message>
<xml_diff>
--- a/docs/03-specs/examples/bill-of-lading-examples.xlsx
+++ b/docs/03-specs/examples/bill-of-lading-examples.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\CAPSTONE\copy\docs\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\CAPSTONE\copy\docs\03-specs\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BB3CED-C08D-4280-9E4F-9EF8116AE40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0373CB21-5D55-4CB8-A819-7882197E737A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>